<commit_message>
version 0.2 added multiple figs and grid
</commit_message>
<xml_diff>
--- a/db/National worksheet.xlsx
+++ b/db/National worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorri\OneDrive\Work\Aus Energy Model Paul Zeba\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6726EE71-2B78-47BD-9184-AE93C0DC913F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9B946D-7EC5-4B32-BAB7-A9B255AD2BC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A46" sqref="A45:XFD46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3356,7 +3356,7 @@
         <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
         <v>71</v>

</xml_diff>